<commit_message>
Added Spark Extent Reports
</commit_message>
<xml_diff>
--- a/src/test/resources/test-result/mobile-details.xlsx
+++ b/src/test/resources/test-result/mobile-details.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="84">
   <si>
     <t>null</t>
   </si>
@@ -217,6 +217,54 @@
   </si>
   <si>
     <t>458</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M13 5G (Stardust Brown, 4GB, 64GB Storage) | 5000mAh Battery | Upto 8GB RAM with RAM Plus</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M53 5G (Deep Ocean Blue, 6GB, 128GB Storage) | 108MP | sAmoled+ 120Hz | 12GB RAM with RAM Plus | Travel Adapter to be Purchased Separately</t>
+  </si>
+  <si>
+    <t>21,999</t>
+  </si>
+  <si>
+    <t>60,900</t>
+  </si>
+  <si>
+    <t>1,22,999</t>
+  </si>
+  <si>
+    <t>11,699</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M13 5G (Aqua Green, 4GB, 64GB Storage) | 5000mAh Battery | Upto 8GB RAM with RAM Plus</t>
+  </si>
+  <si>
+    <t>9,699</t>
+  </si>
+  <si>
+    <t>34,999</t>
+  </si>
+  <si>
+    <t>IKALL Z1 4G Smartphone with Android 8.1 (4GB RAM, 5.5 Inch Display) (Blue)</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14 Pro 128GB Deep Purple</t>
+  </si>
+  <si>
+    <t>10,499</t>
+  </si>
+  <si>
+    <t>Redmi Note 12 5G Matte Black 6GB RAM 128GB ROM | 1st Phone with 120Hz Super AMOLED and Snapdragon® 4 Gen 1 | 48MP AI Triple Camera</t>
+  </si>
+  <si>
+    <t>19,999</t>
+  </si>
+  <si>
+    <t>74,900</t>
+  </si>
+  <si>
+    <t>Apple iPhone 12 (256GB) - White</t>
   </si>
 </sst>
 </file>
@@ -485,18 +533,18 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -504,7 +552,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +560,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -520,15 +568,15 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -536,71 +584,71 @@
         <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">
@@ -608,23 +656,23 @@
         <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20">
@@ -632,39 +680,39 @@
         <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
@@ -672,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Property File Utiltiy and used the same in TestBase
</commit_message>
<xml_diff>
--- a/src/test/resources/test-result/mobile-details.xlsx
+++ b/src/test/resources/test-result/mobile-details.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="89">
   <si>
     <t>null</t>
   </si>
@@ -265,6 +265,21 @@
   </si>
   <si>
     <t>Apple iPhone 12 (256GB) - White</t>
+  </si>
+  <si>
+    <t>59,900</t>
+  </si>
+  <si>
+    <t>79,999</t>
+  </si>
+  <si>
+    <t>478</t>
+  </si>
+  <si>
+    <t>67,039</t>
+  </si>
+  <si>
+    <t>10,999</t>
   </si>
 </sst>
 </file>
@@ -533,18 +548,18 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -552,7 +567,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -560,7 +575,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -568,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -576,7 +591,7 @@
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8">
@@ -584,7 +599,7 @@
         <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -592,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -600,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
@@ -608,23 +623,23 @@
         <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -632,15 +647,15 @@
         <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -648,12 +663,12 @@
         <v>38</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>45</v>
@@ -661,58 +676,58 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
@@ -720,7 +735,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>